<commit_message>
exif metadata issue skipped for now, only data from FileInfo class available for now
</commit_message>
<xml_diff>
--- a/Documentation/metadata_directory_types.xlsx
+++ b/Documentation/metadata_directory_types.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ludwi\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f8993c4f9875f6c3/SourceCode/C^N/PicturePerfect/Documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4C25D6C-E833-4A09-9C0F-8FD6708DC174}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="13_ncr:1_{D4C25D6C-E833-4A09-9C0F-8FD6708DC174}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9AB6FF18-F25E-4210-85BA-DE12A1EDD2C3}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="23">
   <si>
     <t>ORF</t>
   </si>
@@ -88,6 +88,12 @@
   </si>
   <si>
     <t>HuffmanTablesDirectory</t>
+  </si>
+  <si>
+    <t>https://en.wikipedia.org/wiki/Exif</t>
+  </si>
+  <si>
+    <t>Tags and values</t>
   </si>
 </sst>
 </file>
@@ -338,6 +344,50 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:oneCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>1656783</xdr:colOff>
+      <xdr:row>79</xdr:row>
+      <xdr:rowOff>17905</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6A49401A-D629-4FA9-8B37-C394FA420782}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2876550" y="6029325"/>
+          <a:ext cx="4533333" cy="9161905"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -604,10 +654,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:C38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -627,7 +677,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -655,7 +705,7 @@
       <c r="B4" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>3</v>
       </c>
     </row>
@@ -663,7 +713,7 @@
       <c r="A5" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="3" t="s">
         <v>3</v>
       </c>
       <c r="C5" s="4" t="s">
@@ -758,19 +808,34 @@
         <v>17</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B17" s="4" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B18" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B19" s="3" t="s">
         <v>13</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>

</xml_diff>